<commit_message>
treatment added for CDDEM in helix
</commit_message>
<xml_diff>
--- a/tmee/data_in/data_dictionary/indicator_dictionary_TM_v7.xlsx
+++ b/tmee/data_in/data_dictionary/indicator_dictionary_TM_v7.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Snapshot" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7509" uniqueCount="3595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7510" uniqueCount="3595">
   <si>
     <t>snapshot_id</t>
   </si>
@@ -10251,9 +10251,6 @@
     <t>CDDEM_D18</t>
   </si>
   <si>
-    <t>Do not ETL: Extracted by causes independently</t>
-  </si>
-  <si>
     <t>Detailed causes of under-five deaths (x 15)</t>
   </si>
   <si>
@@ -10828,6 +10825,9 @@
   </si>
   <si>
     <t>SN-314</t>
+  </si>
+  <si>
+    <t>Do not ETL: CDDEM helix source extracted outside ETL API loop</t>
   </si>
 </sst>
 </file>
@@ -11617,7 +11617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A296" workbookViewId="0">
+    <sheetView topLeftCell="A56" workbookViewId="0">
       <selection activeCell="G312" sqref="G312"/>
     </sheetView>
   </sheetViews>
@@ -21451,7 +21451,7 @@
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A290" s="1" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
       <c r="B290" s="16" t="s">
         <v>1459</v>
@@ -21475,7 +21475,7 @@
         <v>PCNT</v>
       </c>
       <c r="H290" s="1" t="s">
-        <v>3539</v>
+        <v>3538</v>
       </c>
       <c r="I290" s="25" t="str">
         <f>VLOOKUP(H290,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21485,7 +21485,7 @@
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A291" s="1" t="s">
-        <v>3569</v>
+        <v>3568</v>
       </c>
       <c r="B291" s="16" t="s">
         <v>1461</v>
@@ -21509,7 +21509,7 @@
         <v>PCNT</v>
       </c>
       <c r="H291" s="1" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
       <c r="I291" s="25" t="str">
         <f>VLOOKUP(H291,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21519,7 +21519,7 @@
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A292" s="1" t="s">
-        <v>3570</v>
+        <v>3569</v>
       </c>
       <c r="B292" s="16" t="s">
         <v>1463</v>
@@ -21543,7 +21543,7 @@
         <v>PCNT</v>
       </c>
       <c r="H292" s="1" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
       <c r="I292" s="25" t="str">
         <f>VLOOKUP(H292,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21553,7 +21553,7 @@
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A293" s="1" t="s">
-        <v>3571</v>
+        <v>3570</v>
       </c>
       <c r="B293" s="16" t="s">
         <v>1465</v>
@@ -21577,7 +21577,7 @@
         <v>PCNT</v>
       </c>
       <c r="H293" s="1" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
       <c r="I293" s="25" t="str">
         <f>VLOOKUP(H293,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21587,7 +21587,7 @@
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A294" s="1" t="s">
-        <v>3572</v>
+        <v>3571</v>
       </c>
       <c r="B294" s="16" t="s">
         <v>1466</v>
@@ -21611,7 +21611,7 @@
         <v>PCNT</v>
       </c>
       <c r="H294" s="1" t="s">
-        <v>3543</v>
+        <v>3542</v>
       </c>
       <c r="I294" s="25" t="str">
         <f>VLOOKUP(H294,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21621,7 +21621,7 @@
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A295" s="1" t="s">
-        <v>3573</v>
+        <v>3572</v>
       </c>
       <c r="B295" s="16" t="s">
         <v>1468</v>
@@ -21645,7 +21645,7 @@
         <v>PCNT</v>
       </c>
       <c r="H295" s="1" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="I295" s="25" t="str">
         <f>VLOOKUP(H295,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21655,7 +21655,7 @@
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A296" s="1" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
       <c r="B296" s="16" t="s">
         <v>1470</v>
@@ -21679,7 +21679,7 @@
         <v>PCNT</v>
       </c>
       <c r="H296" s="1" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
       <c r="I296" s="25" t="str">
         <f>VLOOKUP(H296,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21689,7 +21689,7 @@
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A297" s="1" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="B297" s="16" t="s">
         <v>1472</v>
@@ -21713,7 +21713,7 @@
         <v>PCNT</v>
       </c>
       <c r="H297" s="1" t="s">
-        <v>3546</v>
+        <v>3545</v>
       </c>
       <c r="I297" s="25" t="str">
         <f>VLOOKUP(H297,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21723,7 +21723,7 @@
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A298" s="1" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
       <c r="B298" s="16" t="s">
         <v>1474</v>
@@ -21747,7 +21747,7 @@
         <v>PCNT</v>
       </c>
       <c r="H298" s="1" t="s">
-        <v>3547</v>
+        <v>3546</v>
       </c>
       <c r="I298" s="25" t="str">
         <f>VLOOKUP(H298,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21757,7 +21757,7 @@
     </row>
     <row r="299" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A299" s="1" t="s">
-        <v>3577</v>
+        <v>3576</v>
       </c>
       <c r="B299" s="16" t="s">
         <v>1476</v>
@@ -21781,7 +21781,7 @@
         <v>PCNT</v>
       </c>
       <c r="H299" s="1" t="s">
-        <v>3548</v>
+        <v>3547</v>
       </c>
       <c r="I299" s="25" t="str">
         <f>VLOOKUP(H299,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21791,7 +21791,7 @@
     </row>
     <row r="300" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A300" s="1" t="s">
-        <v>3578</v>
+        <v>3577</v>
       </c>
       <c r="B300" s="16" t="s">
         <v>1478</v>
@@ -21815,7 +21815,7 @@
         <v>PCNT</v>
       </c>
       <c r="H300" s="1" t="s">
-        <v>3549</v>
+        <v>3548</v>
       </c>
       <c r="I300" s="25" t="str">
         <f>VLOOKUP(H300,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21825,7 +21825,7 @@
     </row>
     <row r="301" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A301" s="1" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="B301" s="16" t="s">
         <v>1480</v>
@@ -21849,7 +21849,7 @@
         <v>PCNT</v>
       </c>
       <c r="H301" s="1" t="s">
-        <v>3550</v>
+        <v>3549</v>
       </c>
       <c r="I301" s="25" t="str">
         <f>VLOOKUP(H301,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21859,7 +21859,7 @@
     </row>
     <row r="302" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A302" s="1" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="B302" s="16" t="s">
         <v>1482</v>
@@ -21883,7 +21883,7 @@
         <v>PCNT</v>
       </c>
       <c r="H302" s="1" t="s">
-        <v>3551</v>
+        <v>3550</v>
       </c>
       <c r="I302" s="25" t="str">
         <f>VLOOKUP(H302,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21893,7 +21893,7 @@
     </row>
     <row r="303" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A303" s="1" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
       <c r="B303" s="16" t="s">
         <v>1484</v>
@@ -21917,7 +21917,7 @@
         <v>PCNT</v>
       </c>
       <c r="H303" s="1" t="s">
-        <v>3552</v>
+        <v>3551</v>
       </c>
       <c r="I303" s="25" t="str">
         <f>VLOOKUP(H303,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21927,7 +21927,7 @@
     </row>
     <row r="304" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A304" s="1" t="s">
-        <v>3582</v>
+        <v>3581</v>
       </c>
       <c r="B304" s="16" t="s">
         <v>1486</v>
@@ -21951,7 +21951,7 @@
         <v>PCNT</v>
       </c>
       <c r="H304" s="1" t="s">
-        <v>3553</v>
+        <v>3552</v>
       </c>
       <c r="I304" s="25" t="str">
         <f>VLOOKUP(H304,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21961,7 +21961,7 @@
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A305" s="1" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="B305" s="16" t="s">
         <v>1488</v>
@@ -21985,7 +21985,7 @@
         <v>PCNT</v>
       </c>
       <c r="H305" s="1" t="s">
-        <v>3554</v>
+        <v>3553</v>
       </c>
       <c r="I305" s="25" t="str">
         <f>VLOOKUP(H305,Source!$A$2:$G$313,3,FALSE)</f>
@@ -21995,7 +21995,7 @@
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A306" s="1" t="s">
-        <v>3584</v>
+        <v>3583</v>
       </c>
       <c r="B306" s="16" t="s">
         <v>1490</v>
@@ -22019,7 +22019,7 @@
         <v>PCNT</v>
       </c>
       <c r="H306" s="1" t="s">
-        <v>3555</v>
+        <v>3554</v>
       </c>
       <c r="I306" s="25" t="str">
         <f>VLOOKUP(H306,Source!$A$2:$G$385,3,FALSE)</f>
@@ -22029,7 +22029,7 @@
     </row>
     <row r="307" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A307" s="1" t="s">
-        <v>3585</v>
+        <v>3584</v>
       </c>
       <c r="B307" s="16" t="s">
         <v>1492</v>
@@ -22053,7 +22053,7 @@
         <v>PCNT</v>
       </c>
       <c r="H307" s="1" t="s">
-        <v>3556</v>
+        <v>3555</v>
       </c>
       <c r="I307" s="25" t="str">
         <f>VLOOKUP(H307,Source!$A$2:$G$385,3,FALSE)</f>
@@ -22063,7 +22063,7 @@
     </row>
     <row r="308" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A308" s="1" t="s">
-        <v>3586</v>
+        <v>3585</v>
       </c>
       <c r="B308" s="16" t="s">
         <v>1494</v>
@@ -22087,7 +22087,7 @@
         <v>NUMBER</v>
       </c>
       <c r="H308" s="1" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
       <c r="I308" s="25" t="str">
         <f>VLOOKUP(H308,Source!$A$2:$G$385,3,FALSE)</f>
@@ -22097,7 +22097,7 @@
     </row>
     <row r="309" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A309" s="1" t="s">
-        <v>3587</v>
+        <v>3586</v>
       </c>
       <c r="B309" s="16" t="s">
         <v>1496</v>
@@ -22121,7 +22121,7 @@
         <v>NUMBER</v>
       </c>
       <c r="H309" s="1" t="s">
-        <v>3558</v>
+        <v>3557</v>
       </c>
       <c r="I309" s="25" t="str">
         <f>VLOOKUP(H309,Source!$A$2:$G$385,3,FALSE)</f>
@@ -22131,7 +22131,7 @@
     </row>
     <row r="310" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A310" s="1" t="s">
-        <v>3588</v>
+        <v>3587</v>
       </c>
       <c r="B310" s="16" t="s">
         <v>1498</v>
@@ -22155,7 +22155,7 @@
         <v>NUMBER</v>
       </c>
       <c r="H310" s="1" t="s">
-        <v>3559</v>
+        <v>3558</v>
       </c>
       <c r="I310" s="25" t="str">
         <f>VLOOKUP(H310,Source!$A$2:$G$385,3,FALSE)</f>
@@ -22165,7 +22165,7 @@
     </row>
     <row r="311" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A311" s="1" t="s">
-        <v>3589</v>
+        <v>3588</v>
       </c>
       <c r="B311" s="16" t="s">
         <v>1500</v>
@@ -22189,7 +22189,7 @@
         <v>NUMBER</v>
       </c>
       <c r="H311" s="1" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="I311" s="25" t="str">
         <f>VLOOKUP(H311,Source!$A$2:$G$385,3,FALSE)</f>
@@ -22199,7 +22199,7 @@
     </row>
     <row r="312" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A312" s="1" t="s">
-        <v>3590</v>
+        <v>3589</v>
       </c>
       <c r="B312" s="16" t="s">
         <v>1501</v>
@@ -22223,7 +22223,7 @@
         <v>PCNT</v>
       </c>
       <c r="H312" s="1" t="s">
-        <v>3561</v>
+        <v>3560</v>
       </c>
       <c r="I312" s="25" t="str">
         <f>VLOOKUP(H312,Source!$A$2:$G$385,3,FALSE)</f>
@@ -22233,7 +22233,7 @@
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A314" s="1" t="s">
-        <v>3591</v>
+        <v>3590</v>
       </c>
       <c r="B314" s="16" t="s">
         <v>1607</v>
@@ -22257,7 +22257,7 @@
         <v>PCNT</v>
       </c>
       <c r="H314" s="1" t="s">
-        <v>3562</v>
+        <v>3561</v>
       </c>
       <c r="I314" s="25" t="str">
         <f>VLOOKUP(H314,Source!$A$2:$G$330,3,FALSE)</f>
@@ -22266,7 +22266,7 @@
     </row>
     <row r="315" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A315" s="1" t="s">
-        <v>3592</v>
+        <v>3591</v>
       </c>
       <c r="B315" s="16" t="s">
         <v>1611</v>
@@ -22290,7 +22290,7 @@
         <v>PCNT</v>
       </c>
       <c r="H315" s="1" t="s">
-        <v>3563</v>
+        <v>3562</v>
       </c>
       <c r="I315" s="25" t="str">
         <f>VLOOKUP(H315,Source!$A$2:$G$330,3,FALSE)</f>
@@ -22299,7 +22299,7 @@
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A316" s="1" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
       <c r="B316" s="16" t="s">
         <v>2735</v>
@@ -22323,7 +22323,7 @@
         <v>BINARY</v>
       </c>
       <c r="H316" s="1" t="s">
-        <v>3564</v>
+        <v>3563</v>
       </c>
       <c r="I316" s="25" t="str">
         <f>VLOOKUP(H316,Source!$A$2:$G$330,3,FALSE)</f>
@@ -22332,7 +22332,7 @@
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A317" s="1" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
       <c r="B317" s="16" t="s">
         <v>2736</v>
@@ -22356,7 +22356,7 @@
         <v>BINARY</v>
       </c>
       <c r="H317" s="1" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="I317" s="25" t="str">
         <f>VLOOKUP(H317,Source!$A$2:$G$330,3,FALSE)</f>
@@ -22900,9 +22900,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M737"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A371" sqref="A371:A737"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M86" sqref="M86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23961,7 +23961,7 @@
         <v>1993</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>3467</v>
+        <v>3466</v>
       </c>
       <c r="E47" s="44" t="s">
         <v>2756</v>
@@ -24081,7 +24081,7 @@
         <v>1993</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>3467</v>
+        <v>3466</v>
       </c>
       <c r="E53" s="44" t="s">
         <v>2753</v>
@@ -24187,7 +24187,7 @@
         <v>1993</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>3461</v>
+        <v>3460</v>
       </c>
       <c r="E58" s="44" t="s">
         <v>2759</v>
@@ -24353,7 +24353,7 @@
         <v>1993</v>
       </c>
       <c r="D66" s="25" t="s">
-        <v>3438</v>
+        <v>3437</v>
       </c>
       <c r="E66" s="44" t="s">
         <v>2799</v>
@@ -24399,7 +24399,7 @@
         <v>1993</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>3438</v>
+        <v>3437</v>
       </c>
       <c r="E68" s="44" t="s">
         <v>2801</v>
@@ -24422,7 +24422,7 @@
         <v>1993</v>
       </c>
       <c r="D69" s="25" t="s">
-        <v>3438</v>
+        <v>3437</v>
       </c>
       <c r="E69" s="44" t="s">
         <v>2802</v>
@@ -24705,7 +24705,7 @@
         <v>3391</v>
       </c>
       <c r="E82" s="44" t="s">
-        <v>3411</v>
+        <v>3410</v>
       </c>
       <c r="F82" t="s">
         <v>3392</v>
@@ -24765,13 +24765,13 @@
         <v>3391</v>
       </c>
       <c r="E85" s="45" t="s">
-        <v>3403</v>
+        <v>3402</v>
       </c>
       <c r="F85" t="s">
         <v>3401</v>
       </c>
       <c r="M85" s="37" t="s">
-        <v>3402</v>
+        <v>3594</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
@@ -24788,10 +24788,10 @@
         <v>3391</v>
       </c>
       <c r="E86" s="45" t="s">
-        <v>3412</v>
+        <v>3411</v>
       </c>
       <c r="F86" t="s">
-        <v>3406</v>
+        <v>3405</v>
       </c>
       <c r="M86" s="36"/>
     </row>
@@ -24806,13 +24806,13 @@
         <v>1993</v>
       </c>
       <c r="D87" t="s">
+        <v>3412</v>
+      </c>
+      <c r="E87" s="45" t="s">
+        <v>3416</v>
+      </c>
+      <c r="F87" t="s">
         <v>3413</v>
-      </c>
-      <c r="E87" s="45" t="s">
-        <v>3417</v>
-      </c>
-      <c r="F87" t="s">
-        <v>3414</v>
       </c>
       <c r="M87" s="36"/>
     </row>
@@ -24827,13 +24827,13 @@
         <v>1993</v>
       </c>
       <c r="D88" t="s">
-        <v>3413</v>
+        <v>3412</v>
       </c>
       <c r="E88" s="45" t="s">
-        <v>3418</v>
+        <v>3417</v>
       </c>
       <c r="F88" t="s">
-        <v>3428</v>
+        <v>3427</v>
       </c>
       <c r="M88" s="36"/>
     </row>
@@ -24848,13 +24848,13 @@
         <v>1993</v>
       </c>
       <c r="D89" t="s">
-        <v>3413</v>
+        <v>3412</v>
       </c>
       <c r="E89" s="45" t="s">
-        <v>3419</v>
+        <v>3418</v>
       </c>
       <c r="F89" t="s">
-        <v>3429</v>
+        <v>3428</v>
       </c>
       <c r="M89" s="36"/>
     </row>
@@ -24869,13 +24869,13 @@
         <v>1993</v>
       </c>
       <c r="D90" t="s">
-        <v>3413</v>
+        <v>3412</v>
       </c>
       <c r="E90" s="45" t="s">
-        <v>3420</v>
+        <v>3419</v>
       </c>
       <c r="F90" t="s">
-        <v>3430</v>
+        <v>3429</v>
       </c>
       <c r="M90" s="36"/>
     </row>
@@ -24890,13 +24890,13 @@
         <v>1993</v>
       </c>
       <c r="D91" t="s">
-        <v>3413</v>
+        <v>3412</v>
       </c>
       <c r="E91" s="45" t="s">
-        <v>3432</v>
+        <v>3431</v>
       </c>
       <c r="F91" t="s">
-        <v>3431</v>
+        <v>3430</v>
       </c>
       <c r="M91" s="36"/>
     </row>
@@ -24911,13 +24911,13 @@
         <v>1993</v>
       </c>
       <c r="D92" t="s">
-        <v>3413</v>
+        <v>3412</v>
       </c>
       <c r="E92" s="45" t="s">
-        <v>3436</v>
+        <v>3435</v>
       </c>
       <c r="F92" t="s">
-        <v>3435</v>
+        <v>3434</v>
       </c>
       <c r="M92" s="36"/>
     </row>
@@ -24932,13 +24932,13 @@
         <v>1993</v>
       </c>
       <c r="D93" t="s">
+        <v>3437</v>
+      </c>
+      <c r="E93" s="45" t="s">
+        <v>3439</v>
+      </c>
+      <c r="F93" t="s">
         <v>3438</v>
-      </c>
-      <c r="E93" s="45" t="s">
-        <v>3440</v>
-      </c>
-      <c r="F93" t="s">
-        <v>3439</v>
       </c>
       <c r="M93" s="36"/>
     </row>
@@ -24953,13 +24953,13 @@
         <v>1993</v>
       </c>
       <c r="D94" t="s">
-        <v>3438</v>
+        <v>3437</v>
       </c>
       <c r="E94" s="45" t="s">
-        <v>3444</v>
+        <v>3443</v>
       </c>
       <c r="F94" t="s">
-        <v>3447</v>
+        <v>3446</v>
       </c>
       <c r="M94" s="36"/>
     </row>
@@ -24974,13 +24974,13 @@
         <v>1993</v>
       </c>
       <c r="D95" t="s">
-        <v>3438</v>
+        <v>3437</v>
       </c>
       <c r="E95" s="45" t="s">
-        <v>3445</v>
+        <v>3444</v>
       </c>
       <c r="F95" t="s">
-        <v>3448</v>
+        <v>3447</v>
       </c>
       <c r="M95" s="36"/>
     </row>
@@ -24995,13 +24995,13 @@
         <v>1993</v>
       </c>
       <c r="D96" t="s">
-        <v>3438</v>
+        <v>3437</v>
       </c>
       <c r="E96" s="45" t="s">
-        <v>3446</v>
+        <v>3445</v>
       </c>
       <c r="F96" t="s">
-        <v>3449</v>
+        <v>3448</v>
       </c>
       <c r="M96" s="36"/>
     </row>
@@ -25016,13 +25016,13 @@
         <v>1993</v>
       </c>
       <c r="D97" t="s">
-        <v>3438</v>
+        <v>3437</v>
       </c>
       <c r="E97" s="45" t="s">
-        <v>3458</v>
+        <v>3457</v>
       </c>
       <c r="F97" t="s">
-        <v>3457</v>
+        <v>3456</v>
       </c>
       <c r="M97" s="36"/>
     </row>
@@ -25037,15 +25037,17 @@
         <v>1993</v>
       </c>
       <c r="D98" t="s">
+        <v>3460</v>
+      </c>
+      <c r="E98" s="45" t="s">
         <v>3461</v>
       </c>
-      <c r="E98" s="45" t="s">
-        <v>3462</v>
-      </c>
       <c r="F98" t="s">
-        <v>3464</v>
-      </c>
-      <c r="M98" s="36"/>
+        <v>3463</v>
+      </c>
+      <c r="M98" s="37" t="s">
+        <v>3594</v>
+      </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="16" t="s">
@@ -25058,13 +25060,13 @@
         <v>1993</v>
       </c>
       <c r="D99" t="s">
-        <v>3461</v>
+        <v>3460</v>
       </c>
       <c r="E99" s="45" t="s">
-        <v>3466</v>
+        <v>3465</v>
       </c>
       <c r="F99" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="M99" s="36"/>
     </row>
@@ -25079,13 +25081,13 @@
         <v>1993</v>
       </c>
       <c r="D100" t="s">
+        <v>3466</v>
+      </c>
+      <c r="E100" s="45" t="s">
+        <v>3470</v>
+      </c>
+      <c r="F100" t="s">
         <v>3467</v>
-      </c>
-      <c r="E100" s="45" t="s">
-        <v>3471</v>
-      </c>
-      <c r="F100" t="s">
-        <v>3468</v>
       </c>
       <c r="M100" s="36"/>
     </row>
@@ -25100,13 +25102,13 @@
         <v>1993</v>
       </c>
       <c r="D101" t="s">
-        <v>3467</v>
+        <v>3466</v>
       </c>
       <c r="E101" s="45" t="s">
-        <v>3507</v>
+        <v>3506</v>
       </c>
       <c r="F101" t="s">
-        <v>3472</v>
+        <v>3471</v>
       </c>
       <c r="M101" s="36"/>
     </row>
@@ -25121,13 +25123,13 @@
         <v>1993</v>
       </c>
       <c r="D102" t="s">
-        <v>3467</v>
+        <v>3466</v>
       </c>
       <c r="E102" s="45" t="s">
-        <v>3508</v>
+        <v>3507</v>
       </c>
       <c r="F102" t="s">
-        <v>3475</v>
+        <v>3474</v>
       </c>
       <c r="M102" s="36"/>
     </row>
@@ -25142,13 +25144,13 @@
         <v>1993</v>
       </c>
       <c r="D103" t="s">
-        <v>3467</v>
+        <v>3466</v>
       </c>
       <c r="E103" s="45" t="s">
-        <v>3482</v>
+        <v>3481</v>
       </c>
       <c r="F103" t="s">
-        <v>3477</v>
+        <v>3476</v>
       </c>
       <c r="M103" s="36"/>
     </row>
@@ -25163,13 +25165,13 @@
         <v>1993</v>
       </c>
       <c r="D104" t="s">
-        <v>3467</v>
+        <v>3466</v>
       </c>
       <c r="E104" s="45" t="s">
-        <v>3481</v>
+        <v>3480</v>
       </c>
       <c r="F104" t="s">
-        <v>3479</v>
+        <v>3478</v>
       </c>
       <c r="M104" s="36"/>
     </row>
@@ -25184,13 +25186,13 @@
         <v>1993</v>
       </c>
       <c r="D105" t="s">
-        <v>3467</v>
+        <v>3466</v>
       </c>
       <c r="E105" s="45" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
       <c r="F105" t="s">
-        <v>3483</v>
+        <v>3482</v>
       </c>
       <c r="M105" s="36"/>
     </row>
@@ -25205,13 +25207,13 @@
         <v>1993</v>
       </c>
       <c r="D106" t="s">
-        <v>3467</v>
+        <v>3466</v>
       </c>
       <c r="E106" s="45" t="s">
-        <v>3488</v>
+        <v>3487</v>
       </c>
       <c r="F106" t="s">
-        <v>3486</v>
+        <v>3485</v>
       </c>
       <c r="M106" s="36"/>
     </row>
@@ -25226,13 +25228,13 @@
         <v>1993</v>
       </c>
       <c r="D107" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
       <c r="E107" s="45" t="s">
-        <v>3498</v>
+        <v>3497</v>
       </c>
       <c r="F107" t="s">
-        <v>3489</v>
+        <v>3488</v>
       </c>
       <c r="M107" s="36"/>
     </row>
@@ -25247,13 +25249,13 @@
         <v>1993</v>
       </c>
       <c r="D108" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
       <c r="E108" s="45" t="s">
-        <v>3495</v>
+        <v>3494</v>
       </c>
       <c r="F108" t="s">
-        <v>3494</v>
+        <v>3493</v>
       </c>
       <c r="M108" s="36"/>
     </row>
@@ -25268,13 +25270,13 @@
         <v>1993</v>
       </c>
       <c r="D109" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
       <c r="E109" s="45" t="s">
-        <v>3497</v>
+        <v>3496</v>
       </c>
       <c r="F109" t="s">
-        <v>3496</v>
+        <v>3495</v>
       </c>
       <c r="M109" s="36"/>
     </row>
@@ -25289,13 +25291,13 @@
         <v>1993</v>
       </c>
       <c r="D110" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
       <c r="E110" s="45" t="s">
-        <v>3509</v>
+        <v>3508</v>
       </c>
       <c r="F110" t="s">
-        <v>3499</v>
+        <v>3498</v>
       </c>
       <c r="M110" s="36"/>
     </row>
@@ -34054,7 +34056,7 @@
     </row>
     <row r="709" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A709" s="16" t="s">
-        <v>3510</v>
+        <v>3509</v>
       </c>
       <c r="E709" t="s">
         <v>1906</v>
@@ -34064,7 +34066,7 @@
     </row>
     <row r="710" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A710" s="16" t="s">
-        <v>3511</v>
+        <v>3510</v>
       </c>
       <c r="E710" t="s">
         <v>1908</v>
@@ -34074,7 +34076,7 @@
     </row>
     <row r="711" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A711" s="16" t="s">
-        <v>3512</v>
+        <v>3511</v>
       </c>
       <c r="E711" t="s">
         <v>1910</v>
@@ -34084,7 +34086,7 @@
     </row>
     <row r="712" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A712" s="16" t="s">
-        <v>3513</v>
+        <v>3512</v>
       </c>
       <c r="E712" t="s">
         <v>1912</v>
@@ -34094,7 +34096,7 @@
     </row>
     <row r="713" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A713" s="16" t="s">
-        <v>3514</v>
+        <v>3513</v>
       </c>
       <c r="E713" t="s">
         <v>1914</v>
@@ -34104,7 +34106,7 @@
     </row>
     <row r="714" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A714" s="16" t="s">
-        <v>3515</v>
+        <v>3514</v>
       </c>
       <c r="E714" t="s">
         <v>1916</v>
@@ -34114,7 +34116,7 @@
     </row>
     <row r="715" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A715" s="16" t="s">
-        <v>3516</v>
+        <v>3515</v>
       </c>
       <c r="E715" t="s">
         <v>1918</v>
@@ -34124,7 +34126,7 @@
     </row>
     <row r="716" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A716" s="16" t="s">
-        <v>3517</v>
+        <v>3516</v>
       </c>
       <c r="E716" t="s">
         <v>1920</v>
@@ -34134,7 +34136,7 @@
     </row>
     <row r="717" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A717" s="16" t="s">
-        <v>3518</v>
+        <v>3517</v>
       </c>
       <c r="E717" t="s">
         <v>1922</v>
@@ -34144,7 +34146,7 @@
     </row>
     <row r="718" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A718" s="16" t="s">
-        <v>3519</v>
+        <v>3518</v>
       </c>
       <c r="E718" t="s">
         <v>1924</v>
@@ -34152,7 +34154,7 @@
     </row>
     <row r="719" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A719" s="16" t="s">
-        <v>3520</v>
+        <v>3519</v>
       </c>
       <c r="E719" t="s">
         <v>1926</v>
@@ -34160,7 +34162,7 @@
     </row>
     <row r="720" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A720" s="16" t="s">
-        <v>3521</v>
+        <v>3520</v>
       </c>
       <c r="E720" t="s">
         <v>1928</v>
@@ -34168,7 +34170,7 @@
     </row>
     <row r="721" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A721" s="16" t="s">
-        <v>3522</v>
+        <v>3521</v>
       </c>
       <c r="E721" t="s">
         <v>1930</v>
@@ -34176,7 +34178,7 @@
     </row>
     <row r="722" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A722" s="16" t="s">
-        <v>3523</v>
+        <v>3522</v>
       </c>
       <c r="E722" t="s">
         <v>1932</v>
@@ -34184,7 +34186,7 @@
     </row>
     <row r="723" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A723" s="16" t="s">
-        <v>3524</v>
+        <v>3523</v>
       </c>
       <c r="E723" t="s">
         <v>1936</v>
@@ -34192,7 +34194,7 @@
     </row>
     <row r="724" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A724" s="16" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="E724" t="s">
         <v>1938</v>
@@ -34200,7 +34202,7 @@
     </row>
     <row r="725" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A725" s="16" t="s">
-        <v>3526</v>
+        <v>3525</v>
       </c>
       <c r="E725" t="s">
         <v>1940</v>
@@ -34208,7 +34210,7 @@
     </row>
     <row r="726" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A726" s="16" t="s">
-        <v>3527</v>
+        <v>3526</v>
       </c>
       <c r="E726" t="s">
         <v>1942</v>
@@ -34216,7 +34218,7 @@
     </row>
     <row r="727" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A727" s="16" t="s">
-        <v>3528</v>
+        <v>3527</v>
       </c>
       <c r="E727" t="s">
         <v>1944</v>
@@ -34224,7 +34226,7 @@
     </row>
     <row r="728" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A728" s="16" t="s">
-        <v>3529</v>
+        <v>3528</v>
       </c>
       <c r="E728" t="s">
         <v>1946</v>
@@ -34234,7 +34236,7 @@
     </row>
     <row r="729" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A729" s="16" t="s">
-        <v>3530</v>
+        <v>3529</v>
       </c>
       <c r="E729" t="s">
         <v>1948</v>
@@ -34244,7 +34246,7 @@
     </row>
     <row r="730" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A730" s="16" t="s">
-        <v>3531</v>
+        <v>3530</v>
       </c>
       <c r="E730" t="s">
         <v>1950</v>
@@ -34254,7 +34256,7 @@
     </row>
     <row r="731" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A731" s="16" t="s">
-        <v>3532</v>
+        <v>3531</v>
       </c>
       <c r="E731" t="s">
         <v>1952</v>
@@ -34264,7 +34266,7 @@
     </row>
     <row r="732" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A732" s="16" t="s">
-        <v>3533</v>
+        <v>3532</v>
       </c>
       <c r="E732" t="s">
         <v>1954</v>
@@ -34274,7 +34276,7 @@
     </row>
     <row r="733" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A733" s="16" t="s">
-        <v>3534</v>
+        <v>3533</v>
       </c>
       <c r="E733" t="s">
         <v>1956</v>
@@ -34290,7 +34292,7 @@
     </row>
     <row r="734" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A734" s="16" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="E734" t="s">
         <v>2819</v>
@@ -34303,7 +34305,7 @@
     </row>
     <row r="735" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A735" s="16" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
       <c r="E735" t="s">
         <v>1958</v>
@@ -34316,7 +34318,7 @@
     </row>
     <row r="736" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A736" s="16" t="s">
-        <v>3537</v>
+        <v>3536</v>
       </c>
       <c r="E736" t="s">
         <v>1960</v>
@@ -34326,7 +34328,7 @@
     </row>
     <row r="737" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A737" s="16" t="s">
-        <v>3538</v>
+        <v>3537</v>
       </c>
       <c r="E737" t="s">
         <v>1962</v>
@@ -35235,10 +35237,10 @@
         <v>2481</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>3408</v>
+      </c>
+      <c r="H43" s="25" t="s">
         <v>3409</v>
-      </c>
-      <c r="H43" s="25" t="s">
-        <v>3410</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -35255,7 +35257,7 @@
         <v>2330</v>
       </c>
       <c r="H44" s="25" t="s">
-        <v>3505</v>
+        <v>3504</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -35272,7 +35274,7 @@
         <v>2320</v>
       </c>
       <c r="H45" s="25" t="s">
-        <v>3506</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -35595,7 +35597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K327"/>
   <sheetViews>
-    <sheetView topLeftCell="A309" workbookViewId="0">
+    <sheetView topLeftCell="A54" workbookViewId="0">
       <selection activeCell="A322" sqref="A322:A327"/>
     </sheetView>
   </sheetViews>
@@ -37160,10 +37162,10 @@
         <v>2154</v>
       </c>
       <c r="C55" s="46" t="s">
+        <v>3403</v>
+      </c>
+      <c r="D55" s="24" t="s">
         <v>3404</v>
-      </c>
-      <c r="D55" s="24" t="s">
-        <v>3405</v>
       </c>
       <c r="E55" t="s">
         <v>2153</v>
@@ -37189,10 +37191,10 @@
         <v>639</v>
       </c>
       <c r="C56" s="46" t="s">
+        <v>3406</v>
+      </c>
+      <c r="D56" s="24" t="s">
         <v>3407</v>
-      </c>
-      <c r="D56" s="24" t="s">
-        <v>3408</v>
       </c>
       <c r="E56" t="s">
         <v>2153</v>
@@ -37218,10 +37220,10 @@
         <v>639</v>
       </c>
       <c r="C57" s="46" t="s">
+        <v>3414</v>
+      </c>
+      <c r="D57" s="24" t="s">
         <v>3415</v>
-      </c>
-      <c r="D57" s="24" t="s">
-        <v>3416</v>
       </c>
       <c r="E57" t="s">
         <v>2153</v>
@@ -37233,7 +37235,7 @@
         <v>2021</v>
       </c>
       <c r="I57" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
       <c r="J57" t="s">
         <v>643</v>
@@ -37247,10 +37249,10 @@
         <v>639</v>
       </c>
       <c r="C58" s="46" t="s">
+        <v>3425</v>
+      </c>
+      <c r="D58" s="24" t="s">
         <v>3426</v>
-      </c>
-      <c r="D58" s="24" t="s">
-        <v>3427</v>
       </c>
       <c r="E58" t="s">
         <v>2153</v>
@@ -37262,7 +37264,7 @@
         <v>2021</v>
       </c>
       <c r="I58" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
       <c r="J58" t="s">
         <v>643</v>
@@ -37276,10 +37278,10 @@
         <v>639</v>
       </c>
       <c r="C59" s="46" t="s">
+        <v>3421</v>
+      </c>
+      <c r="D59" s="24" t="s">
         <v>3422</v>
-      </c>
-      <c r="D59" s="24" t="s">
-        <v>3423</v>
       </c>
       <c r="E59" t="s">
         <v>2153</v>
@@ -37291,7 +37293,7 @@
         <v>2021</v>
       </c>
       <c r="I59" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
       <c r="J59" t="s">
         <v>643</v>
@@ -37305,10 +37307,10 @@
         <v>639</v>
       </c>
       <c r="C60" s="46" t="s">
-        <v>3425</v>
+        <v>3424</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>3424</v>
+        <v>3423</v>
       </c>
       <c r="E60" t="s">
         <v>2153</v>
@@ -37320,7 +37322,7 @@
         <v>2021</v>
       </c>
       <c r="I60" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
       <c r="J60" t="s">
         <v>643</v>
@@ -37334,10 +37336,10 @@
         <v>639</v>
       </c>
       <c r="C61" s="46" t="s">
+        <v>3432</v>
+      </c>
+      <c r="D61" t="s">
         <v>3433</v>
-      </c>
-      <c r="D61" t="s">
-        <v>3434</v>
       </c>
       <c r="E61" t="s">
         <v>2153</v>
@@ -37363,7 +37365,7 @@
         <v>2195</v>
       </c>
       <c r="C62" s="46" t="s">
-        <v>3437</v>
+        <v>3436</v>
       </c>
       <c r="D62" s="24" t="s">
         <v>2197</v>
@@ -37392,10 +37394,10 @@
         <v>639</v>
       </c>
       <c r="C63" s="46" t="s">
+        <v>3440</v>
+      </c>
+      <c r="D63" s="24" t="s">
         <v>3441</v>
-      </c>
-      <c r="D63" s="24" t="s">
-        <v>3442</v>
       </c>
       <c r="E63" t="s">
         <v>2153</v>
@@ -37407,7 +37409,7 @@
         <v>2021</v>
       </c>
       <c r="I63" t="s">
-        <v>3443</v>
+        <v>3442</v>
       </c>
       <c r="J63" t="s">
         <v>643</v>
@@ -37421,10 +37423,10 @@
         <v>639</v>
       </c>
       <c r="C64" s="46" t="s">
-        <v>3450</v>
+        <v>3449</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>3453</v>
+        <v>3452</v>
       </c>
       <c r="E64" t="s">
         <v>2153</v>
@@ -37436,7 +37438,7 @@
         <v>2021</v>
       </c>
       <c r="I64" t="s">
-        <v>3456</v>
+        <v>3455</v>
       </c>
       <c r="J64" t="s">
         <v>643</v>
@@ -37450,10 +37452,10 @@
         <v>639</v>
       </c>
       <c r="C65" s="46" t="s">
-        <v>3451</v>
+        <v>3450</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>3454</v>
+        <v>3453</v>
       </c>
       <c r="E65" t="s">
         <v>2153</v>
@@ -37465,7 +37467,7 @@
         <v>2021</v>
       </c>
       <c r="I65" t="s">
-        <v>3456</v>
+        <v>3455</v>
       </c>
       <c r="J65" t="s">
         <v>643</v>
@@ -37479,10 +37481,10 @@
         <v>639</v>
       </c>
       <c r="C66" s="46" t="s">
-        <v>3452</v>
+        <v>3451</v>
       </c>
       <c r="D66" s="24" t="s">
-        <v>3455</v>
+        <v>3454</v>
       </c>
       <c r="E66" t="s">
         <v>2153</v>
@@ -37494,7 +37496,7 @@
         <v>2021</v>
       </c>
       <c r="I66" t="s">
-        <v>3456</v>
+        <v>3455</v>
       </c>
       <c r="J66" t="s">
         <v>643</v>
@@ -37508,10 +37510,10 @@
         <v>639</v>
       </c>
       <c r="C67" s="46" t="s">
+        <v>3458</v>
+      </c>
+      <c r="D67" t="s">
         <v>3459</v>
-      </c>
-      <c r="D67" t="s">
-        <v>3460</v>
       </c>
       <c r="E67" t="s">
         <v>2153</v>
@@ -37537,10 +37539,10 @@
         <v>2154</v>
       </c>
       <c r="C68" s="46" t="s">
-        <v>3463</v>
+        <v>3462</v>
       </c>
       <c r="D68" t="s">
-        <v>3405</v>
+        <v>3404</v>
       </c>
       <c r="E68" t="s">
         <v>2153</v>
@@ -37566,10 +37568,10 @@
         <v>639</v>
       </c>
       <c r="C69" s="46" t="s">
+        <v>3502</v>
+      </c>
+      <c r="D69" s="24" t="s">
         <v>3503</v>
-      </c>
-      <c r="D69" s="24" t="s">
-        <v>3504</v>
       </c>
       <c r="E69" t="s">
         <v>2153</v>
@@ -37581,7 +37583,7 @@
         <v>2021</v>
       </c>
       <c r="I69" t="s">
-        <v>3465</v>
+        <v>3464</v>
       </c>
       <c r="J69" t="s">
         <v>643</v>
@@ -37595,10 +37597,10 @@
         <v>639</v>
       </c>
       <c r="C70" s="46" t="s">
+        <v>3468</v>
+      </c>
+      <c r="D70" s="24" t="s">
         <v>3469</v>
-      </c>
-      <c r="D70" s="24" t="s">
-        <v>3470</v>
       </c>
       <c r="E70" t="s">
         <v>2191</v>
@@ -37624,10 +37626,10 @@
         <v>639</v>
       </c>
       <c r="C71" s="46" t="s">
+        <v>3472</v>
+      </c>
+      <c r="D71" t="s">
         <v>3473</v>
-      </c>
-      <c r="D71" t="s">
-        <v>3474</v>
       </c>
       <c r="E71" t="s">
         <v>2153</v>
@@ -37653,10 +37655,10 @@
         <v>639</v>
       </c>
       <c r="C72" s="46" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
       <c r="D72" t="s">
-        <v>3474</v>
+        <v>3473</v>
       </c>
       <c r="E72" t="s">
         <v>2153</v>
@@ -37682,10 +37684,10 @@
         <v>639</v>
       </c>
       <c r="C73" s="46" t="s">
-        <v>3478</v>
+        <v>3477</v>
       </c>
       <c r="D73" t="s">
-        <v>3474</v>
+        <v>3473</v>
       </c>
       <c r="E73" t="s">
         <v>2153</v>
@@ -37711,10 +37713,10 @@
         <v>639</v>
       </c>
       <c r="C74" s="46" t="s">
-        <v>3480</v>
+        <v>3479</v>
       </c>
       <c r="D74" t="s">
-        <v>3474</v>
+        <v>3473</v>
       </c>
       <c r="E74" t="s">
         <v>2153</v>
@@ -37740,10 +37742,10 @@
         <v>639</v>
       </c>
       <c r="C75" s="46" t="s">
-        <v>3484</v>
+        <v>3483</v>
       </c>
       <c r="D75" t="s">
-        <v>3474</v>
+        <v>3473</v>
       </c>
       <c r="E75" t="s">
         <v>2153</v>
@@ -37769,10 +37771,10 @@
         <v>639</v>
       </c>
       <c r="C76" s="46" t="s">
-        <v>3487</v>
+        <v>3486</v>
       </c>
       <c r="D76" t="s">
-        <v>3474</v>
+        <v>3473</v>
       </c>
       <c r="E76" t="s">
         <v>2153</v>
@@ -37798,10 +37800,10 @@
         <v>639</v>
       </c>
       <c r="C77" s="46" t="s">
+        <v>3490</v>
+      </c>
+      <c r="D77" t="s">
         <v>3491</v>
-      </c>
-      <c r="D77" t="s">
-        <v>3492</v>
       </c>
       <c r="E77" t="s">
         <v>2153</v>
@@ -37827,10 +37829,10 @@
         <v>639</v>
       </c>
       <c r="C78" s="46" t="s">
-        <v>3493</v>
+        <v>3492</v>
       </c>
       <c r="D78" t="s">
-        <v>3492</v>
+        <v>3491</v>
       </c>
       <c r="E78" t="s">
         <v>2153</v>
@@ -37856,10 +37858,10 @@
         <v>639</v>
       </c>
       <c r="C79" s="46" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
       <c r="D79" t="s">
-        <v>3492</v>
+        <v>3491</v>
       </c>
       <c r="E79" t="s">
         <v>2153</v>
@@ -37885,10 +37887,10 @@
         <v>639</v>
       </c>
       <c r="C80" s="46" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
       <c r="D80" t="s">
-        <v>3492</v>
+        <v>3491</v>
       </c>
       <c r="E80" t="s">
         <v>2153</v>
@@ -44179,7 +44181,7 @@
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A298" s="1" t="s">
-        <v>3539</v>
+        <v>3538</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>639</v>
@@ -44208,7 +44210,7 @@
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A299" s="1" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
       <c r="B299" s="1" t="s">
         <v>639</v>
@@ -44237,7 +44239,7 @@
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A300" s="1" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
       <c r="B300" s="1" t="s">
         <v>639</v>
@@ -44266,7 +44268,7 @@
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A301" s="1" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
       <c r="B301" s="1" t="s">
         <v>639</v>
@@ -44295,7 +44297,7 @@
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A302" s="1" t="s">
-        <v>3543</v>
+        <v>3542</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>639</v>
@@ -44324,7 +44326,7 @@
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A303" s="1" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="B303" s="1" t="s">
         <v>639</v>
@@ -44353,7 +44355,7 @@
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A304" s="1" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>639</v>
@@ -44382,7 +44384,7 @@
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A305" s="1" t="s">
-        <v>3546</v>
+        <v>3545</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>639</v>
@@ -44411,7 +44413,7 @@
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A306" s="1" t="s">
-        <v>3547</v>
+        <v>3546</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>639</v>
@@ -44440,7 +44442,7 @@
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A307" s="1" t="s">
-        <v>3548</v>
+        <v>3547</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>639</v>
@@ -44469,7 +44471,7 @@
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A308" s="1" t="s">
-        <v>3549</v>
+        <v>3548</v>
       </c>
       <c r="B308" s="1" t="s">
         <v>639</v>
@@ -44498,7 +44500,7 @@
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A309" s="1" t="s">
-        <v>3550</v>
+        <v>3549</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>639</v>
@@ -44527,7 +44529,7 @@
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A310" s="1" t="s">
-        <v>3551</v>
+        <v>3550</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>639</v>
@@ -44556,7 +44558,7 @@
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A311" s="1" t="s">
-        <v>3552</v>
+        <v>3551</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>639</v>
@@ -44585,7 +44587,7 @@
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A312" s="1" t="s">
-        <v>3553</v>
+        <v>3552</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>639</v>
@@ -44614,7 +44616,7 @@
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A313" s="1" t="s">
-        <v>3554</v>
+        <v>3553</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>639</v>
@@ -44643,7 +44645,7 @@
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A314" s="1" t="s">
-        <v>3555</v>
+        <v>3554</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>639</v>
@@ -44672,7 +44674,7 @@
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A315" s="1" t="s">
-        <v>3556</v>
+        <v>3555</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>639</v>
@@ -44701,7 +44703,7 @@
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A316" s="1" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>639</v>
@@ -44730,7 +44732,7 @@
     </row>
     <row r="317" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A317" s="1" t="s">
-        <v>3558</v>
+        <v>3557</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>639</v>
@@ -44759,7 +44761,7 @@
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A318" s="1" t="s">
-        <v>3559</v>
+        <v>3558</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>639</v>
@@ -44788,7 +44790,7 @@
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A319" s="1" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>639</v>
@@ -44817,7 +44819,7 @@
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A320" s="1" t="s">
-        <v>3561</v>
+        <v>3560</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>639</v>
@@ -44854,7 +44856,7 @@
     </row>
     <row r="322" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A322" s="1" t="s">
-        <v>3562</v>
+        <v>3561</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>639</v>
@@ -44883,7 +44885,7 @@
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A323" s="1" t="s">
-        <v>3563</v>
+        <v>3562</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>639</v>
@@ -44912,7 +44914,7 @@
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A324" s="1" t="s">
-        <v>3564</v>
+        <v>3563</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>639</v>
@@ -44941,7 +44943,7 @@
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A325" s="1" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>639</v>
@@ -44970,7 +44972,7 @@
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A326" s="1" t="s">
-        <v>3566</v>
+        <v>3565</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>2154</v>
@@ -44996,7 +44998,7 @@
     </row>
     <row r="327" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A327" s="1" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>2154</v>

</xml_diff>